<commit_message>
Adapt Link Trafo example RMIP No
</commit_message>
<xml_diff>
--- a/data/Two_Node_Link/Global_Parameters.xlsx
+++ b/data/Two_Node_Link/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Two_Node_Link\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B080A-484F-47FB-9728-7071140E477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66612176-4D43-49A0-8B5D-B9A5EB393903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>[h]</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -402,11 +405,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -801,27 +804,29 @@
   </sheetPr>
   <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.35546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -841,7 +846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -853,7 +858,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -873,12 +878,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -889,12 +894,12 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -909,12 +914,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
@@ -924,7 +929,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
@@ -936,7 +941,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
@@ -956,12 +961,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
@@ -972,7 +977,7 @@
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
@@ -992,7 +997,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1005,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1016,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1096,12 +1101,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1247,6 +1246,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -1256,22 +1261,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1287,4 +1276,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>